<commit_message>
Update Pendulum Team Hours Worked.xlsx
Updated Worked Hours to Represent Class Time
</commit_message>
<xml_diff>
--- a/Team Files/Hours Worked/Pendulum Team Hours Worked.xlsx
+++ b/Team Files/Hours Worked/Pendulum Team Hours Worked.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbear\OneDrive\Desktop\Pendulum Project\EG-310-InvertedPendulum\Team Files\Hours Worked\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0081ABDA-BB24-49D8-9D6A-AC661979B485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856413C1-CCD6-41CC-9EBC-2932739EF34E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" xr2:uid="{69133C28-2E56-4F40-A366-946EDDA72998}"/>
   </bookViews>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="10">
   <si>
     <t>Team Members Name</t>
   </si>
@@ -60,6 +58,12 @@
   </si>
   <si>
     <t>Kathryn Swineford</t>
+  </si>
+  <si>
+    <t>1/2 - 1/6</t>
+  </si>
+  <si>
+    <t>1/9 - 1/13</t>
   </si>
 </sst>
 </file>
@@ -457,7 +461,7 @@
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -472,10 +476,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -576,10 +580,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="3">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3">
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="D3" s="3">
         <v>0</v>
@@ -629,10 +633,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="3">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="3">
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
@@ -682,7 +686,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="3">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="3">
         <v>0</v>
@@ -735,10 +739,10 @@
         <v>7</v>
       </c>
       <c r="B6" s="3">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="3">
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="D6" s="3">
         <v>0</v>
@@ -859,11 +863,11 @@
       </c>
       <c r="B9" s="3">
         <f>SUM(B3:B7)</f>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ref="C9:Q9" si="0">SUM(C3:C7)</f>
-        <v>0</v>
+        <v>3.75</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Add PDP Draft and Updated Hours Worked
</commit_message>
<xml_diff>
--- a/Team Files/Hours Worked/Pendulum Team Hours Worked.xlsx
+++ b/Team Files/Hours Worked/Pendulum Team Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbear\OneDrive\Desktop\Pendulum Project\EG-310-InvertedPendulum\Team Files\Hours Worked\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3DD128-25FB-4BE5-B8BB-5E4946BCB8AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15477268-A272-4349-A4B0-8816E12480F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" xr2:uid="{69133C28-2E56-4F40-A366-946EDDA72998}"/>
   </bookViews>
@@ -461,7 +461,7 @@
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -589,7 +589,7 @@
         <v>1.25</v>
       </c>
       <c r="E3" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F3" s="3">
         <v>0</v>
@@ -642,7 +642,7 @@
         <v>1.75</v>
       </c>
       <c r="E4" s="3">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="F4" s="3">
         <v>0</v>
@@ -695,7 +695,7 @@
         <v>1.25</v>
       </c>
       <c r="E5" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F5" s="3">
         <v>0</v>
@@ -748,7 +748,7 @@
         <v>1.25</v>
       </c>
       <c r="E6" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F6" s="3">
         <v>0</v>
@@ -798,9 +798,7 @@
       <c r="D7" s="3">
         <v>0</v>
       </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
+      <c r="E7" s="3"/>
       <c r="F7" s="3">
         <v>0</v>
       </c>
@@ -875,7 +873,7 @@
       </c>
       <c r="E9" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="F9" s="3">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
PDP Draft #1, Meeting Minutes, Hours Worked
We finished PDP Draft #1 today.
I updated the meeting minutes and hours worked to reflect this.
</commit_message>
<xml_diff>
--- a/Team Files/Hours Worked/Pendulum Team Hours Worked.xlsx
+++ b/Team Files/Hours Worked/Pendulum Team Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbear\OneDrive\Desktop\Pendulum Project\EG-310-InvertedPendulum\Team Files\Hours Worked\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15477268-A272-4349-A4B0-8816E12480F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C24A694-66B0-46F8-BC54-0F1FC8CDBDA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" xr2:uid="{69133C28-2E56-4F40-A366-946EDDA72998}"/>
   </bookViews>
@@ -461,7 +461,7 @@
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -589,7 +589,7 @@
         <v>1.25</v>
       </c>
       <c r="E3" s="3">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="F3" s="3">
         <v>0</v>
@@ -642,7 +642,7 @@
         <v>1.75</v>
       </c>
       <c r="E4" s="3">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="F4" s="3">
         <v>0</v>
@@ -695,7 +695,7 @@
         <v>1.25</v>
       </c>
       <c r="E5" s="3">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="F5" s="3">
         <v>0</v>
@@ -748,7 +748,7 @@
         <v>1.25</v>
       </c>
       <c r="E6" s="3">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="F6" s="3">
         <v>0</v>
@@ -873,7 +873,7 @@
       </c>
       <c r="E9" s="3">
         <f t="shared" si="0"/>
-        <v>8.5</v>
+        <v>14.5</v>
       </c>
       <c r="F9" s="3">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Added this week's status report
Updated the hours worked document and added this weeks status report!
</commit_message>
<xml_diff>
--- a/Team Files/Hours Worked/Pendulum Team Hours Worked.xlsx
+++ b/Team Files/Hours Worked/Pendulum Team Hours Worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbear\OneDrive\Desktop\Pendulum Project\EG-310-InvertedPendulum\Team Files\Hours Worked\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C24A694-66B0-46F8-BC54-0F1FC8CDBDA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B505511-E011-4461-B340-4FA76ED25A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" xr2:uid="{69133C28-2E56-4F40-A366-946EDDA72998}"/>
   </bookViews>
@@ -461,7 +461,7 @@
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -642,7 +642,7 @@
         <v>1.75</v>
       </c>
       <c r="E4" s="3">
-        <v>4</v>
+        <v>4.25</v>
       </c>
       <c r="F4" s="3">
         <v>0</v>
@@ -873,7 +873,7 @@
       </c>
       <c r="E9" s="3">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>14.75</v>
       </c>
       <c r="F9" s="3">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Feat/pdp draft #1 (#8)
Hey this is great! PDP draft went well, I'm merging this in favor of a new branch.

Co-authored-by: KenwoodFox <kenwood364@gmail.com>
</commit_message>
<xml_diff>
--- a/Team Files/Hours Worked/Pendulum Team Hours Worked.xlsx
+++ b/Team Files/Hours Worked/Pendulum Team Hours Worked.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbear\OneDrive\Desktop\Pendulum Project\EG-310-InvertedPendulum\Team Files\Hours Worked\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0081ABDA-BB24-49D8-9D6A-AC661979B485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B505511-E011-4461-B340-4FA76ED25A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" xr2:uid="{69133C28-2E56-4F40-A366-946EDDA72998}"/>
   </bookViews>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="10">
   <si>
     <t>Team Members Name</t>
   </si>
@@ -60,6 +58,12 @@
   </si>
   <si>
     <t>Kathryn Swineford</t>
+  </si>
+  <si>
+    <t>1/2 - 1/6</t>
+  </si>
+  <si>
+    <t>1/9 - 1/13</t>
   </si>
 </sst>
 </file>
@@ -446,7 +450,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -457,7 +461,7 @@
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -472,10 +476,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -576,16 +580,16 @@
         <v>5</v>
       </c>
       <c r="B3" s="3">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="D3" s="3">
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="E3" s="3">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="F3" s="3">
         <v>0</v>
@@ -629,16 +633,16 @@
         <v>4</v>
       </c>
       <c r="B4" s="3">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="3">
-        <v>0</v>
+        <v>3.25</v>
       </c>
       <c r="D4" s="3">
-        <v>0</v>
+        <v>1.75</v>
       </c>
       <c r="E4" s="3">
-        <v>0</v>
+        <v>4.25</v>
       </c>
       <c r="F4" s="3">
         <v>0</v>
@@ -682,16 +686,16 @@
         <v>6</v>
       </c>
       <c r="B5" s="3">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="3">
         <v>0</v>
       </c>
       <c r="D5" s="3">
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="E5" s="3">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="F5" s="3">
         <v>0</v>
@@ -735,16 +739,16 @@
         <v>7</v>
       </c>
       <c r="B6" s="3">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="3">
-        <v>0</v>
+        <v>3.25</v>
       </c>
       <c r="D6" s="3">
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="E6" s="3">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="F6" s="3">
         <v>0</v>
@@ -794,9 +798,7 @@
       <c r="D7" s="3">
         <v>0</v>
       </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
+      <c r="E7" s="3"/>
       <c r="F7" s="3">
         <v>0</v>
       </c>
@@ -859,19 +861,19 @@
       </c>
       <c r="B9" s="3">
         <f>SUM(B3:B7)</f>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ref="C9:Q9" si="0">SUM(C3:C7)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14.75</v>
       </c>
       <c r="F9" s="3">
         <f t="shared" si="0"/>

</xml_diff>